<commit_message>
Updated Data Dictionary to indicate remaining columns after pre-processing
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjoshi/Documents/LendingClub/Quarterly_Loan_Stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chihongtao/loan_prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1678E574-8418-2242-BAA5-F112E89F91E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$129</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1201,7 +1202,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1384,7 +1385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1567,6 +1568,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1818,7 +1837,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1835,7 +1854,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1856,6 +1874,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2250,15 +2295,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A145" sqref="A145:B145"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2270,39 +2315,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    </row>
+    <row r="3" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
@@ -2313,14 +2355,13 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -2331,88 +2372,81 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+    </row>
+    <row r="9" spans="1:4" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    </row>
+    <row r="10" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+    </row>
+    <row r="11" spans="1:4" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    </row>
+    <row r="12" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+    </row>
+    <row r="13" spans="1:4" s="37" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    </row>
+    <row r="15" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="24"/>
-    </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="C15" s="36"/>
+    </row>
+    <row r="16" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="24"/>
-    </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="36"/>
+    </row>
+    <row r="17" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -2421,14 +2455,13 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
@@ -2439,34 +2472,31 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    </row>
+    <row r="21" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="22" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2475,7 +2505,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2484,50 +2514,46 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="26" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    </row>
+    <row r="27" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    </row>
+    <row r="28" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="24"/>
+      <c r="C29" s="23"/>
     </row>
     <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
@@ -2536,16 +2562,15 @@
       <c r="B30" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C30" s="24"/>
-    </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
@@ -2565,54 +2590,49 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    </row>
+    <row r="35" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    </row>
+    <row r="36" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    </row>
+    <row r="37" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
-    </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+    </row>
+    <row r="38" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2621,7 +2641,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2630,41 +2650,41 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:11" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="D41" s="29"/>
+    </row>
+    <row r="42" spans="1:11" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="D42" s="29"/>
+    </row>
+    <row r="43" spans="1:11" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="D43" s="29"/>
+    </row>
+    <row r="44" spans="1:11" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D44" s="4"/>
+      <c r="D44" s="34"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
@@ -2675,7 +2695,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2687,58 +2707,58 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="39" t="s">
         <v>299</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="9" t="s">
+      <c r="D47" s="37"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="40"/>
+    </row>
+    <row r="48" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
+      <c r="D48" s="37"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+    </row>
+    <row r="49" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+      <c r="D49" s="37"/>
+    </row>
+    <row r="50" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="D50" s="37"/>
+    </row>
+    <row r="51" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="29"/>
+    </row>
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2756,7 +2776,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2783,23 +2803,23 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
+    <row r="57" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
+      <c r="D57" s="29"/>
+    </row>
+    <row r="58" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="4"/>
+      <c r="D58" s="37"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
@@ -2810,7 +2830,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -2819,130 +2839,128 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="9" t="s">
+      <c r="D61" s="29"/>
+    </row>
+    <row r="62" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="27" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
+    <row r="63" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
+    <row r="64" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="27" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
+    <row r="65" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="9" t="s">
+    <row r="66" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="9" t="s">
+    <row r="67" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="27" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
+    <row r="68" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="27" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
+    <row r="69" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="9" t="s">
+    <row r="70" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="27" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
+    <row r="71" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="27" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
+    <row r="72" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="27" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
+    <row r="73" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="C73"/>
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="9" t="s">
+    </row>
+    <row r="74" spans="1:2" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="24" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="28" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>266</v>
       </c>
@@ -2950,7 +2968,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>269</v>
       </c>
@@ -2958,7 +2976,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
         <v>271</v>
       </c>
@@ -2966,7 +2984,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
         <v>335</v>
       </c>
@@ -2974,7 +2992,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>279</v>
       </c>
@@ -2990,39 +3008,39 @@
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9" t="s">
+    <row r="84" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="27" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="9" t="s">
+    <row r="85" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="38" t="s">
         <v>306</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="27" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>129</v>
       </c>
@@ -3030,119 +3048,119 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="9" t="s">
+    <row r="88" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="27" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
+    <row r="91" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="25" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="9" t="s">
+    <row r="95" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="27" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="9" t="s">
+    <row r="98" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B98" s="38" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
+    <row r="99" spans="1:2" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="38" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
+    <row r="100" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="27" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -3166,11 +3184,11 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="9" t="s">
+    <row r="104" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3182,63 +3200,63 @@
         <v>292</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="s">
+    <row r="106" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="27" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
+    <row r="107" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
+    <row r="108" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="28" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
+    <row r="109" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
+    <row r="110" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" s="28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+    <row r="111" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="9" t="s">
+    <row r="112" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B112" s="38" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -3246,11 +3264,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
+    <row r="114" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="28" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3263,122 +3281,122 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="B116" s="18" t="s">
+      <c r="B116" s="17" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="B117" s="18" t="s">
+      <c r="B117" s="17" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="18" t="s">
+      <c r="A118" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="B118" s="18" t="s">
+      <c r="B118" s="17" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="18" t="s">
+      <c r="A119" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="B119" s="18" t="s">
+      <c r="B119" s="17" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="18" t="s">
+      <c r="A120" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="17" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="18" t="s">
+      <c r="A121" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="B121" s="18" t="s">
+      <c r="B121" s="17" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="18" t="s">
+      <c r="A122" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="17" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="18" t="s">
+      <c r="A123" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="B123" s="18" t="s">
+      <c r="B123" s="17" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="18" t="s">
+      <c r="A124" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="B124" s="18" t="s">
+      <c r="B124" s="17" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="18" t="s">
+      <c r="A125" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="B125" s="18" t="s">
+      <c r="B125" s="17" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="18" t="s">
+      <c r="A126" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="B126" s="18" t="s">
+      <c r="B126" s="17" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="18" t="s">
+      <c r="A127" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="B127" s="18" t="s">
+      <c r="B127" s="17" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="18" t="s">
+      <c r="A128" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="B128" s="18" t="s">
+      <c r="B128" s="17" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="18" t="s">
+      <c r="A129" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="B129" s="18" t="s">
+      <c r="B129" s="17" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="9" t="s">
+    <row r="130" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B130" s="9" t="s">
+      <c r="B130" s="38" t="s">
         <v>367</v>
       </c>
     </row>
@@ -3494,19 +3512,19 @@
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="9" t="s">
+    <row r="145" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="38" t="s">
         <v>362</v>
       </c>
-      <c r="B145" s="9" t="s">
+      <c r="B145" s="38" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="9" t="s">
+    <row r="146" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="42" t="s">
         <v>345</v>
       </c>
-      <c r="B146" s="9" t="s">
+      <c r="B146" s="42" t="s">
         <v>337</v>
       </c>
     </row>
@@ -3558,14 +3576,14 @@
         <v>344</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B154" s="13" t="s">
+    <row r="154" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B154" s="12" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B129"/>
-  <sortState ref="A2:B101">
+  <autoFilter ref="A1:B129" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3574,12 +3592,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3590,10 +3608,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3634,7 +3652,7 @@
       <c r="A5" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>241</v>
       </c>
       <c r="D5" s="6"/>
@@ -3809,7 +3827,7 @@
       <c r="A22" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>238</v>
       </c>
       <c r="D22" s="6"/>
@@ -3820,7 +3838,7 @@
       <c r="A23" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>167</v>
       </c>
       <c r="D23" s="6"/>
@@ -4012,7 +4030,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -4617,114 +4635,114 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="22" t="s">
+      <c r="A107" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="B107" s="22" t="s">
+      <c r="B107" s="21" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="18" t="s">
+      <c r="A108" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="B108" s="18" t="s">
+      <c r="B108" s="17" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="18" t="s">
+      <c r="A109" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="B109" s="18" t="s">
+      <c r="B109" s="17" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="18" t="s">
+      <c r="A110" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="17" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="B111" s="18" t="s">
+      <c r="B111" s="17" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="18" t="s">
+      <c r="A112" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="B112" s="18" t="s">
+      <c r="B112" s="17" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="B113" s="18" t="s">
+      <c r="B113" s="17" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="18" t="s">
+      <c r="A114" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="B114" s="18" t="s">
+      <c r="B114" s="17" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="18" t="s">
+      <c r="A115" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="B115" s="18" t="s">
+      <c r="B115" s="17" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="B116" s="18" t="s">
+      <c r="B116" s="17" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="B117" s="18" t="s">
+      <c r="B117" s="17" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="18" t="s">
+      <c r="A118" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="B118" s="18" t="s">
+      <c r="B118" s="17" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="18" t="s">
+      <c r="A119" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="B119" s="18" t="s">
+      <c r="B119" s="17" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="18" t="s">
+      <c r="A120" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="17" t="s">
         <v>334</v>
       </c>
     </row>
@@ -4736,18 +4754,18 @@
         <v>382</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B123" s="13" t="s">
+    <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B123" s="12" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B89">
-    <sortState ref="A2:B107">
+  <autoFilter ref="A1:B89" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B107">
       <sortCondition ref="A1:A107"/>
     </sortState>
   </autoFilter>
-  <sortState ref="D2:D93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D93">
     <sortCondition ref="D53:D144"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4756,7 +4774,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4770,95 +4788,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B10"/>
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Data Pre-processing done. Issue to be fixed - x_train & x_test do not have the same number of columns after one-hot encoding
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chihongtao/loan_prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1678E574-8418-2242-BAA5-F112E89F91E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2B3FD8-7E26-9B42-8B52-C962F3BA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37260" yWindow="-800" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -2301,9 +2301,9 @@
   </sheetPr>
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3072,11 +3072,11 @@
         <v>237</v>
       </c>
     </row>
-    <row r="90" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="27" t="s">
+    <row r="90" spans="1:2" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="28" t="s">
+      <c r="B90" s="32" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added few more models: KNN, Logistic Regression, Random Forest, GBM. Also updated Data Dictionary by highlighting key features (based on Decision Tree result) in Green
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chihongtao/loan_prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2B3FD8-7E26-9B42-8B52-C962F3BA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3097403A-8FD5-8341-A069-473EDAF3FBA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37260" yWindow="-800" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="388">
   <si>
     <t>id</t>
   </si>
@@ -1197,6 +1197,21 @@
   </si>
   <si>
     <t>The method by which the borrower receives their loan. Possible values are: CASH, DIRECT_PAY</t>
+  </si>
+  <si>
+    <t>issue_y</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Added col</t>
+  </si>
+  <si>
+    <t>issue_m</t>
+  </si>
+  <si>
+    <t>loan_to_income_ratio</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1400,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1586,6 +1601,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1837,7 +1858,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1891,7 +1912,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1901,6 +1921,18 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2299,11 +2331,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:K159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2322,27 +2354,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="46" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="46" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:4" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="43" t="s">
         <v>241</v>
       </c>
     </row>
@@ -2355,11 +2387,11 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:4" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="43" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2381,7 +2413,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>114</v>
       </c>
       <c r="B9" s="27" t="s">
@@ -2389,30 +2421,30 @@
       </c>
     </row>
     <row r="10" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>296</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:4" s="44" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
         <v>297</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="38" t="s">
+    <row r="12" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="42" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="37" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>226</v>
       </c>
@@ -2420,31 +2452,31 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+    <row r="14" spans="1:4" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+    <row r="15" spans="1:4" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="48"/>
     </row>
     <row r="16" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>298</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -2455,11 +2487,11 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+    <row r="18" spans="1:3" s="44" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="43" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2472,19 +2504,19 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+    <row r="20" spans="1:3" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="43" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+    <row r="21" spans="1:3" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="43" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2530,19 +2562,19 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+    <row r="27" spans="1:3" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="43" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+    <row r="28" spans="1:3" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="43" t="s">
         <v>309</v>
       </c>
     </row>
@@ -2564,7 +2596,7 @@
       </c>
       <c r="C30" s="23"/>
     </row>
-    <row r="31" spans="1:3" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>34</v>
       </c>
@@ -2614,21 +2646,21 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="27" t="s">
+    <row r="37" spans="1:11" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-    </row>
-    <row r="38" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="27" t="s">
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+    </row>
+    <row r="38" spans="1:11" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="43" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2659,23 +2691,23 @@
       </c>
       <c r="D41" s="29"/>
     </row>
-    <row r="42" spans="1:11" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="27" t="s">
+    <row r="42" spans="1:11" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="D42" s="29"/>
-    </row>
-    <row r="43" spans="1:11" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27" t="s">
+      <c r="D42" s="44"/>
+    </row>
+    <row r="43" spans="1:11" s="47" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="29"/>
+      <c r="D43" s="44"/>
     </row>
     <row r="44" spans="1:11" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="31" t="s">
@@ -2708,55 +2740,55 @@
       <c r="K46" s="11"/>
     </row>
     <row r="47" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="38" t="s">
         <v>299</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="37"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
+      <c r="D47" s="36"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
     </row>
     <row r="48" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="38" t="s">
         <v>124</v>
       </c>
       <c r="B48" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="37"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
+      <c r="D48" s="36"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="39"/>
     </row>
     <row r="49" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="38" t="s">
         <v>125</v>
       </c>
       <c r="B49" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="37"/>
+      <c r="D49" s="36"/>
     </row>
     <row r="50" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="38" t="s">
         <v>111</v>
       </c>
       <c r="B50" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="37"/>
-    </row>
-    <row r="51" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="38" t="s">
+      <c r="D50" s="36"/>
+    </row>
+    <row r="51" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="46" t="s">
         <v>300</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="29"/>
+      <c r="D51" s="44"/>
     </row>
     <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
@@ -2804,7 +2836,7 @@
       <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="38" t="s">
+      <c r="A57" s="37" t="s">
         <v>302</v>
       </c>
       <c r="B57" s="27" t="s">
@@ -2813,13 +2845,13 @@
       <c r="D57" s="29"/>
     </row>
     <row r="58" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="38" t="s">
         <v>304</v>
       </c>
       <c r="B58" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="37"/>
+      <c r="D58" s="36"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
@@ -2839,33 +2871,33 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="38" t="s">
+    <row r="61" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="27" t="s">
+      <c r="B61" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="29"/>
+      <c r="D61" s="44"/>
     </row>
     <row r="62" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="38" t="s">
+      <c r="A62" s="37" t="s">
         <v>116</v>
       </c>
       <c r="B62" s="27" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="38" t="s">
+    <row r="63" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="27" t="s">
+      <c r="B63" s="42" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="38" t="s">
+      <c r="A64" s="37" t="s">
         <v>117</v>
       </c>
       <c r="B64" s="27" t="s">
@@ -2876,7 +2908,7 @@
       <c r="A65" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="27" t="s">
+      <c r="B65" s="24" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2884,7 +2916,7 @@
       <c r="A66" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B66" s="27" t="s">
+      <c r="B66" s="24" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2892,7 +2924,7 @@
       <c r="A67" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="24" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2900,12 +2932,12 @@
       <c r="A68" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="27" t="s">
+      <c r="B68" s="24" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="38" t="s">
+      <c r="A69" s="37" t="s">
         <v>126</v>
       </c>
       <c r="B69" s="27" t="s">
@@ -2913,7 +2945,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="38" t="s">
+      <c r="A70" s="37" t="s">
         <v>109</v>
       </c>
       <c r="B70" s="27" t="s">
@@ -2921,31 +2953,31 @@
       </c>
     </row>
     <row r="71" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="38" t="s">
+      <c r="A71" s="37" t="s">
         <v>121</v>
       </c>
       <c r="B71" s="27" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="38" t="s">
+    <row r="72" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="B72" s="27" t="s">
+      <c r="B72" s="42" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="38" t="s">
+    <row r="73" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B73" s="27" t="s">
+      <c r="B73" s="42" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:2" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="38" t="s">
         <v>110</v>
       </c>
       <c r="B74" s="24" t="s">
@@ -3008,11 +3040,11 @@
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="27" t="s">
+    <row r="82" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="43" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3024,16 +3056,16 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="38" t="s">
+    <row r="84" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B84" s="27" t="s">
+      <c r="B84" s="42" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="38" t="s">
+      <c r="A85" s="37" t="s">
         <v>306</v>
       </c>
       <c r="B85" s="27" t="s">
@@ -3048,27 +3080,27 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="27" t="s">
+    <row r="87" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B87" s="28" t="s">
+      <c r="B87" s="43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="38" t="s">
+    <row r="88" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="B88" s="42" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="27" t="s">
+    <row r="89" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B89" s="28" t="s">
+      <c r="B89" s="43" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3096,35 +3128,35 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="24" t="s">
+    <row r="93" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B93" s="25" t="s">
+      <c r="B93" s="43" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="27" t="s">
+    <row r="94" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B94" s="28" t="s">
+      <c r="B94" s="43" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="38" t="s">
+    <row r="95" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B95" s="27" t="s">
+      <c r="B95" s="42" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="27" t="s">
+    <row r="96" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B96" s="28" t="s">
+      <c r="B96" s="43" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3136,24 +3168,24 @@
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="38" t="s">
+    <row r="98" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="B98" s="38" t="s">
+      <c r="B98" s="46" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="38" t="s">
+      <c r="A99" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="B99" s="38" t="s">
+      <c r="B99" s="37" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="38" t="s">
+      <c r="A100" s="37" t="s">
         <v>112</v>
       </c>
       <c r="B100" s="27" t="s">
@@ -3169,10 +3201,10 @@
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="24" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3185,7 +3217,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="38" t="s">
+      <c r="A104" s="37" t="s">
         <v>308</v>
       </c>
       <c r="B104" s="27" t="s">
@@ -3201,7 +3233,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="38" t="s">
+      <c r="A106" s="37" t="s">
         <v>100</v>
       </c>
       <c r="B106" s="27" t="s">
@@ -3232,11 +3264,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="27" t="s">
+    <row r="110" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="28" t="s">
+      <c r="B110" s="43" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3248,11 +3280,11 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="38" t="s">
+    <row r="112" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="B112" s="38" t="s">
+      <c r="B112" s="46" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3264,11 +3296,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="27" t="s">
+    <row r="114" spans="1:2" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="42" t="s">
         <v>294</v>
       </c>
-      <c r="B114" s="28" t="s">
+      <c r="B114" s="43" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3392,11 +3424,11 @@
         <v>334</v>
       </c>
     </row>
-    <row r="130" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="38" t="s">
+    <row r="130" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="B130" s="38" t="s">
+      <c r="B130" s="46" t="s">
         <v>367</v>
       </c>
     </row>
@@ -3512,19 +3544,19 @@
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="38" t="s">
+    <row r="145" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="46" t="s">
         <v>362</v>
       </c>
-      <c r="B145" s="38" t="s">
+      <c r="B145" s="46" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="146" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="42" t="s">
+      <c r="A146" s="41" t="s">
         <v>345</v>
       </c>
-      <c r="B146" s="42" t="s">
+      <c r="B146" s="41" t="s">
         <v>337</v>
       </c>
     </row>
@@ -3579,6 +3611,31 @@
     <row r="154" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B154" s="12" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="49" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="47" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="47" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="47" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="47" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SVM, Logistics regression with linear SGD classifier, trying Cross Validation approach
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chihongtao/loan_prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3097403A-8FD5-8341-A069-473EDAF3FBA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A178F9F-C8E1-D943-92DD-39C02DC7AD82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$152</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
@@ -2028,7 +2028,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2328,14 +2337,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2378,7 +2387,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>285</v>
       </c>
@@ -2395,7 +2404,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
@@ -2404,7 +2413,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="29" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>252</v>
       </c>
@@ -2412,7 +2421,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="29" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>114</v>
       </c>
@@ -2420,7 +2429,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="29" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>296</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="36" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>226</v>
       </c>
@@ -2469,7 +2478,7 @@
       </c>
       <c r="C15" s="48"/>
     </row>
-    <row r="16" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="29" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
         <v>298</v>
       </c>
@@ -2478,7 +2487,7 @@
       </c>
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -2495,7 +2504,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>255</v>
       </c>
@@ -2520,7 +2529,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="29" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
@@ -2528,7 +2537,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2537,7 +2546,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2546,7 +2555,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="29" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
         <v>3</v>
       </c>
@@ -2554,7 +2563,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="29" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
         <v>4</v>
       </c>
@@ -2578,7 +2587,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2587,7 +2596,7 @@
       </c>
       <c r="C29" s="23"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>277</v>
       </c>
@@ -2596,7 +2605,7 @@
       </c>
       <c r="C30" s="23"/>
     </row>
-    <row r="31" spans="1:3" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="36" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>34</v>
       </c>
@@ -2604,7 +2613,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>287</v>
       </c>
@@ -2613,7 +2622,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>289</v>
       </c>
@@ -2622,7 +2631,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="29" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
         <v>26</v>
       </c>
@@ -2630,7 +2639,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="29" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
         <v>7</v>
       </c>
@@ -2638,7 +2647,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="29" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
         <v>6</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2673,7 +2682,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2682,7 +2691,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="30" customFormat="1" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
         <v>43</v>
       </c>
@@ -2709,7 +2718,7 @@
       </c>
       <c r="D43" s="44"/>
     </row>
-    <row r="44" spans="1:11" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="33" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="31" t="s">
         <v>14</v>
       </c>
@@ -2718,7 +2727,7 @@
       </c>
       <c r="D44" s="34"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>283</v>
       </c>
@@ -2727,7 +2736,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2739,7 +2748,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="38" t="s">
         <v>299</v>
       </c>
@@ -2751,7 +2760,7 @@
       <c r="J47" s="39"/>
       <c r="K47" s="39"/>
     </row>
-    <row r="48" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="38" t="s">
         <v>124</v>
       </c>
@@ -2763,7 +2772,7 @@
       <c r="J48" s="39"/>
       <c r="K48" s="39"/>
     </row>
-    <row r="49" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="38" t="s">
         <v>125</v>
       </c>
@@ -2772,7 +2781,7 @@
       </c>
       <c r="D49" s="36"/>
     </row>
-    <row r="50" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="38" t="s">
         <v>111</v>
       </c>
@@ -2790,7 +2799,7 @@
       </c>
       <c r="D51" s="44"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2799,7 +2808,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>108</v>
       </c>
@@ -2808,7 +2817,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2817,7 +2826,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>273</v>
       </c>
@@ -2826,7 +2835,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>301</v>
       </c>
@@ -2835,7 +2844,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="37" t="s">
         <v>302</v>
       </c>
@@ -2844,7 +2853,7 @@
       </c>
       <c r="D57" s="29"/>
     </row>
-    <row r="58" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="38" t="s">
         <v>304</v>
       </c>
@@ -2853,7 +2862,7 @@
       </c>
       <c r="D58" s="36"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>305</v>
       </c>
@@ -2862,7 +2871,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="6" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -2880,7 +2889,7 @@
       </c>
       <c r="D61" s="44"/>
     </row>
-    <row r="62" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="37" t="s">
         <v>116</v>
       </c>
@@ -2896,7 +2905,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="37" t="s">
         <v>117</v>
       </c>
@@ -2904,7 +2913,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="38" t="s">
         <v>115</v>
       </c>
@@ -2912,7 +2921,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="38" t="s">
         <v>122</v>
       </c>
@@ -2920,7 +2929,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="38" t="s">
         <v>127</v>
       </c>
@@ -2928,7 +2937,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="38" t="s">
         <v>102</v>
       </c>
@@ -2936,7 +2945,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="37" t="s">
         <v>126</v>
       </c>
@@ -2944,7 +2953,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="37" t="s">
         <v>109</v>
       </c>
@@ -2952,7 +2961,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="37" t="s">
         <v>121</v>
       </c>
@@ -2976,7 +2985,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="38" t="s">
         <v>110</v>
       </c>
@@ -2984,7 +2993,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" s="30" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="27" t="s">
         <v>29</v>
       </c>
@@ -2992,7 +3001,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>266</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>269</v>
       </c>
@@ -3008,7 +3017,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
         <v>271</v>
       </c>
@@ -3016,7 +3025,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
         <v>335</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>279</v>
       </c>
@@ -3032,7 +3041,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>281</v>
       </c>
@@ -3048,7 +3057,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" s="26" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="24" t="s">
         <v>36</v>
       </c>
@@ -3064,7 +3073,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="37" t="s">
         <v>306</v>
       </c>
@@ -3072,7 +3081,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>129</v>
       </c>
@@ -3104,7 +3113,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="90" spans="1:2" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" s="33" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="31" t="s">
         <v>15</v>
       </c>
@@ -3112,7 +3121,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" s="26" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="24" t="s">
         <v>225</v>
       </c>
@@ -3120,7 +3129,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" s="26" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="24" t="s">
         <v>31</v>
       </c>
@@ -3160,7 +3169,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:2" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" s="26" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="24" t="s">
         <v>19</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:2" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" s="30" customFormat="1" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="37" t="s">
         <v>113</v>
       </c>
@@ -3184,7 +3193,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="37" t="s">
         <v>112</v>
       </c>
@@ -3192,7 +3201,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -3200,7 +3209,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="38" t="s">
         <v>307</v>
       </c>
@@ -3208,7 +3217,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>275</v>
       </c>
@@ -3216,7 +3225,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="37" t="s">
         <v>308</v>
       </c>
@@ -3224,7 +3233,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
         <v>293</v>
       </c>
@@ -3232,7 +3241,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="106" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="37" t="s">
         <v>100</v>
       </c>
@@ -3240,7 +3249,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" s="30" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="27" t="s">
         <v>37</v>
       </c>
@@ -3248,7 +3257,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" s="30" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="27" t="s">
         <v>38</v>
       </c>
@@ -3256,7 +3265,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" s="30" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="27" t="s">
         <v>40</v>
       </c>
@@ -3272,7 +3281,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="1:2" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" s="30" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="27" t="s">
         <v>39</v>
       </c>
@@ -3288,7 +3297,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -3304,7 +3313,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>257</v>
       </c>
@@ -3312,7 +3321,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
         <v>247</v>
       </c>
@@ -3320,7 +3329,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
         <v>310</v>
       </c>
@@ -3328,7 +3337,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
         <v>312</v>
       </c>
@@ -3336,7 +3345,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
         <v>314</v>
       </c>
@@ -3344,7 +3353,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
         <v>316</v>
       </c>
@@ -3352,7 +3361,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
         <v>318</v>
       </c>
@@ -3360,7 +3369,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
         <v>320</v>
       </c>
@@ -3368,7 +3377,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
         <v>322</v>
       </c>
@@ -3376,7 +3385,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
         <v>324</v>
       </c>
@@ -3384,7 +3393,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
         <v>336</v>
       </c>
@@ -3392,7 +3401,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
         <v>327</v>
       </c>
@@ -3400,7 +3409,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
         <v>329</v>
       </c>
@@ -3408,7 +3417,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
         <v>331</v>
       </c>
@@ -3416,7 +3425,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
         <v>333</v>
       </c>
@@ -3432,7 +3441,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="9" t="s">
         <v>348</v>
       </c>
@@ -3440,7 +3449,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="9" t="s">
         <v>349</v>
       </c>
@@ -3448,7 +3457,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="9" t="s">
         <v>350</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="9" t="s">
         <v>351</v>
       </c>
@@ -3464,7 +3473,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="9" t="s">
         <v>352</v>
       </c>
@@ -3472,7 +3481,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="9" t="s">
         <v>353</v>
       </c>
@@ -3480,7 +3489,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="9" t="s">
         <v>354</v>
       </c>
@@ -3488,7 +3497,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="9" t="s">
         <v>355</v>
       </c>
@@ -3496,7 +3505,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="9" t="s">
         <v>356</v>
       </c>
@@ -3504,7 +3513,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="9" t="s">
         <v>357</v>
       </c>
@@ -3512,7 +3521,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="9" t="s">
         <v>358</v>
       </c>
@@ -3520,7 +3529,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="9" t="s">
         <v>359</v>
       </c>
@@ -3528,7 +3537,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="9" t="s">
         <v>360</v>
       </c>
@@ -3536,7 +3545,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>361</v>
       </c>
@@ -3552,7 +3561,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="146" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" s="33" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="41" t="s">
         <v>345</v>
       </c>
@@ -3560,7 +3569,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="9" t="s">
         <v>346</v>
       </c>
@@ -3568,7 +3577,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="9" t="s">
         <v>363</v>
       </c>
@@ -3576,7 +3585,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
         <v>340</v>
       </c>
@@ -3584,7 +3593,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="9" t="s">
         <v>364</v>
       </c>
@@ -3592,7 +3601,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="9" t="s">
         <v>365</v>
       </c>
@@ -3600,7 +3609,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="9" t="s">
         <v>366</v>
       </c>
@@ -3639,7 +3648,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B129" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B152" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>

</xml_diff>